<commit_message>
adding sample answer sheet
</commit_message>
<xml_diff>
--- a/data/sheets/moving_smoothing_average.xlsx
+++ b/data/sheets/moving_smoothing_average.xlsx
@@ -188,7 +188,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -220,6 +220,30 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="458"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="464"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="491"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -10482,11 +10506,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="45535653"/>
-        <c:axId val="99115092"/>
+        <c:axId val="55336891"/>
+        <c:axId val="22829405"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45535653"/>
+        <c:axId val="55336891"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10521,14 +10545,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99115092"/>
+        <c:crossAx val="22829405"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99115092"/>
+        <c:axId val="22829405"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10572,7 +10596,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45535653"/>
+        <c:crossAx val="55336891"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10619,8 +10643,8 @@
       <xdr:rowOff>38160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>574920</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>128880</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>114840</xdr:rowOff>
     </xdr:to>
@@ -10631,7 +10655,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1665360" y="38160"/>
-        <a:ext cx="15165360" cy="8042040"/>
+        <a:ext cx="15532200" cy="8042040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">

</xml_diff>